<commit_message>
feat(supplier): implement Excel file upload for supplier import
</commit_message>
<xml_diff>
--- a/week 8/jobsheet/public/template_supplier.xlsx
+++ b/week 8/jobsheet/public/template_supplier.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Apps\laragon\www\PWL2025\week 8\jobsheet\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A385A6-607C-4BB9-A0A5-DB4B97F2A7AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FFB0387-25AD-44B1-BF29-47709BFBEBEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{E011ABB6-7838-4C25-A9AE-C084FEA0212F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E011ABB6-7838-4C25-A9AE-C084FEA0212F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,114 +34,111 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Andi Pratama</t>
   </si>
   <si>
-    <t xml:space="preserve"> supplier_kode</t>
+    <t>supplier_kode</t>
+  </si>
+  <si>
+    <t>supplier_nama</t>
+  </si>
+  <si>
+    <t>supplier_alamat</t>
+  </si>
+  <si>
+    <t>supplier_telp</t>
+  </si>
+  <si>
+    <t>supplier_email</t>
+  </si>
+  <si>
+    <t>supplier_kontak</t>
   </si>
   <si>
     <t>SUP006</t>
   </si>
   <si>
+    <t>PT. Teknologi Nusantara</t>
+  </si>
+  <si>
+    <t>Jl. Merdeka No. 88, Yogyakarta</t>
+  </si>
+  <si>
+    <t>0274-1234567</t>
+  </si>
+  <si>
+    <t>info@teknologinusantara.com</t>
+  </si>
+  <si>
+    <t>Rina Susanti</t>
+  </si>
+  <si>
+    <t>SUP007</t>
+  </si>
+  <si>
+    <t>CV. Sumber Makmur</t>
+  </si>
+  <si>
+    <t>Jl. Raya Bogor No. 15, Bogor</t>
+  </si>
+  <si>
+    <t>0251-9876543</t>
+  </si>
+  <si>
+    <t>sales@sumbermakmur.co.id</t>
+  </si>
+  <si>
+    <t>SUP008</t>
+  </si>
+  <si>
+    <t>PT. Jaya Abadi</t>
+  </si>
+  <si>
+    <t>Jl. Sudirman No. 99, Medan</t>
+  </si>
+  <si>
+    <t>061-5557890</t>
+  </si>
+  <si>
+    <t>contact@jayaabadi.com</t>
+  </si>
+  <si>
+    <t>Siti Aminah</t>
+  </si>
+  <si>
     <t>SUP009</t>
   </si>
   <si>
-    <t>SUP007</t>
-  </si>
-  <si>
-    <t>SUP008</t>
+    <t>UD. Cahaya Baru</t>
+  </si>
+  <si>
+    <t>Jl. Diponegoro No. 22, Denpasar</t>
+  </si>
+  <si>
+    <t>0361-4567890</t>
+  </si>
+  <si>
+    <t>order@cahayabaru.com</t>
+  </si>
+  <si>
+    <t>I Made Wirawan</t>
   </si>
   <si>
     <t>SUP010</t>
   </si>
   <si>
-    <t>supplier_nama</t>
-  </si>
-  <si>
-    <t>PT. Teknologi Maju</t>
-  </si>
-  <si>
-    <t>CV. Sumber Makmur</t>
-  </si>
-  <si>
-    <t>UD. Jaya Abadi</t>
-  </si>
-  <si>
-    <t>PT. Cahaya Sentosa</t>
-  </si>
-  <si>
-    <t>CV. Prima Sejahtera</t>
-  </si>
-  <si>
-    <t>supplier_alamat</t>
-  </si>
-  <si>
-    <t>Jl. Inovasi No. 10, Surabaya</t>
-  </si>
-  <si>
-    <t>Jl. Raya No. 88, Yogyakarta</t>
-  </si>
-  <si>
-    <t>Jl. Merdeka No. 15, Medan</t>
-  </si>
-  <si>
-    <t>Jl. Industri Baru No. 22, Bekasi</t>
-  </si>
-  <si>
-    <t>Jl. Pahlawan No. 33, Semarang</t>
-  </si>
-  <si>
-    <t>supplier_telp</t>
-  </si>
-  <si>
-    <t>081-23456789</t>
-  </si>
-  <si>
-    <t>082-34567890</t>
-  </si>
-  <si>
-    <t>085-45678901</t>
-  </si>
-  <si>
-    <t>081-56789012</t>
-  </si>
-  <si>
-    <t>087-67890123</t>
-  </si>
-  <si>
-    <t>supplier_email</t>
-  </si>
-  <si>
-    <t>info@teknologimaju.co.id</t>
-  </si>
-  <si>
-    <t>info@primasejahtera.co.id</t>
-  </si>
-  <si>
-    <t>sales@sumbermakmur.co.id</t>
-  </si>
-  <si>
-    <t>order@jayaabadi.com</t>
-  </si>
-  <si>
-    <t>cs@cahayasentosa.co.id</t>
-  </si>
-  <si>
-    <t>supplier_kontak</t>
-  </si>
-  <si>
-    <t>Rina Susanti</t>
-  </si>
-  <si>
-    <t>Budi Hartono</t>
-  </si>
-  <si>
-    <t>Siti Aminah</t>
-  </si>
-  <si>
-    <t>Dedi Kurniawan</t>
+    <t>PT. Sentosa Raya</t>
+  </si>
+  <si>
+    <t>Jl. Gatot Subroto No. 77, Makassar</t>
+  </si>
+  <si>
+    <t>0411-6543210</t>
+  </si>
+  <si>
+    <t>info@sentosaraya.com</t>
   </si>
 </sst>
 </file>
@@ -194,7 +191,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -203,9 +200,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -523,180 +517,138 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C7E09C-F67F-4A03-912A-0D38297E12F3}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-    </row>
-    <row r="2" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="4"/>
-    </row>
-    <row r="3" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="4"/>
-    </row>
-    <row r="4" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="2"/>
-    </row>
-    <row r="5" spans="1:13" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="2"/>
-    </row>
-    <row r="6" spans="1:13" ht="72" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1" xr:uid="{44C4FB83-BD72-4A2C-8620-FE83E67567F6}"/>
-    <hyperlink ref="E5" r:id="rId2" xr:uid="{642AFA2F-B282-4D4C-B632-071E405CC084}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{292B7A0B-259F-4927-B6D1-CE648E0A81A9}"/>
-    <hyperlink ref="E3" r:id="rId4" xr:uid="{B746ACF0-C3CE-49FE-8820-74504F16A372}"/>
-    <hyperlink ref="E2" r:id="rId5" xr:uid="{886E4847-790C-4BAD-BED7-92968E1D655D}"/>
+    <hyperlink ref="E2" r:id="rId1" display="mailto:info@teknologinusantara.com" xr:uid="{47CF4BCC-D9C2-4620-9BB9-2EE8FF0A8695}"/>
+    <hyperlink ref="E3" r:id="rId2" display="mailto:sales@sumbermakmur.co.id" xr:uid="{3F373B25-1DC0-43B5-BF76-28411C84905A}"/>
+    <hyperlink ref="E4" r:id="rId3" display="mailto:contact@jayaabadi.com" xr:uid="{A9D4DAA5-4FD0-4224-AACA-912B3991BC5F}"/>
+    <hyperlink ref="E5" r:id="rId4" display="mailto:order@cahayabaru.com" xr:uid="{A4818C08-23C3-4EEC-837E-58C40B347540}"/>
+    <hyperlink ref="E6" r:id="rId5" display="mailto:info@sentosaraya.com" xr:uid="{D181DC5C-53D2-448D-8B18-3203B9D60045}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>